<commit_message>
Commit du projet et de la doc
- Ajout de la page d'affichage du menu
- Ajout des méthodes GET
</commit_message>
<xml_diff>
--- a/docs/PHAM_Journal_2025.xlsx
+++ b/docs/PHAM_Journal_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/esther_pham_studentfr_ch/Documents/4eme/TPI/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="13_ncr:1_{5F69E96A-935C-4229-A8D9-62578036D2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAC1B1A2-9C3E-43E7-8958-811352FFE160}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="13_ncr:1_{5F69E96A-935C-4229-A8D9-62578036D2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D0E4056-E3D5-4B8E-9976-56919EA60628}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Journal!$A$6:$HI$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal!$B:$D,Journal!$1:$6</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$G$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Documentation du chapitre 2.1.3 (Processus d’entreprise concernés)</t>
   </si>
   <si>
-    <t>Pendant la visite des experts, on m'a expliqué qu'il faut que je documente bien et que ce soit complet. Il faut que je fasse attention aussi à bien remplir mon journal de travail et mon planning. Je pense que pour le planning, comme ils me l'ont fait remarquer, je dois faire attention pendant la création des services CRUD, cela va prendre plus de temps.</t>
-  </si>
-  <si>
     <t>Création desdiagrammes d'activités</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>Visite du supérieur : Discussion des schémas d'analyse et des modifications à faire. Validation des schémas</t>
   </si>
   <si>
-    <t>Les schémas m'ont pris énormement de temps sur le planning et maintenant je suis en retard. Il faut absolument que je rattrape ce retard le plus rapidement possible demain.</t>
-  </si>
-  <si>
     <t>Création du diagramme de classes pour le client</t>
   </si>
   <si>
@@ -172,13 +166,43 @@
     <t>Visite du supérieur : Discussion des schémas de conception et modifications à faire</t>
   </si>
   <si>
-    <t>Création de la structure du serveur et connection à la DB</t>
-  </si>
-  <si>
     <t>Conception des tests et documentation des tests</t>
   </si>
   <si>
     <t>Création des différentes requêtes GET et documentation des schémas</t>
+  </si>
+  <si>
+    <t>Pendant la visite des experts, on m'a expliqué qu'il faut que je documente bien et que ce soit complet. Il faut que je fasse attention aussi à bien remplir mon journal de travail et mon planning. Je pense que pour le planning, comme ils me l'ont fait remarquer, je dois faire attention pendant la création des services CRUD : cela va prendre plus de temps.</t>
+  </si>
+  <si>
+    <t>Les schémas m'ont pris énormément de temps sur le planning, et maintenant je suis en retard. Il faut absolument que je rattrape ce retard le plus rapidement possible demain.</t>
+  </si>
+  <si>
+    <t>J'ai réussi à rattraper mon retard, heureusement, et maintenant je peux me reconcentrer sur les tâches sans trop me stresser. Cela me soulage beaucoup, mais il faut que j'avance sur la documentation aussi, étant donné que je l'ai laissée de côté pour rattraper mon retard.</t>
+  </si>
+  <si>
+    <t>Visite du supérieur :  
+- Discussion des schémas de conception et modifications à faire
+- Discussion des requêtes GET
+- Discussion de la page admin</t>
+  </si>
+  <si>
+    <t>Création des différentes requêtes GET et tests</t>
+  </si>
+  <si>
+    <t>Création de la structure du serveur et connection à la DB ainsi que les tests</t>
+  </si>
+  <si>
+    <t>Création des pages d'affichage des articles</t>
+  </si>
+  <si>
+    <t>Test de l'affichage et de l'animation</t>
+  </si>
+  <si>
+    <t>L'animation des items du menu ne fonctionnait pas et renvoyait soit des erreurs, soit la page n'affichait rien.</t>
+  </si>
+  <si>
+    <t>Il fallait importer les fichiers CSS de la librairie Slick pour que l'animation fonctionne. Il fallait également appliquer l'animation sur la liste et non sur les sections du menu.</t>
   </si>
 </sst>
 </file>
@@ -564,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -633,145 +657,131 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1335,16 +1345,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:D31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="1"/>
-    <col min="2" max="3" width="31.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="28" style="1" customWidth="1"/>
@@ -1416,7 +1427,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18">
+      <c r="A7" s="45">
         <v>45796</v>
       </c>
       <c r="B7" s="40" t="s">
@@ -1428,7 +1439,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="25" t="s">
         <v>11</v>
       </c>
@@ -1438,59 +1449,59 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="27" t="s">
-        <v>24</v>
+      <c r="A14" s="20"/>
+      <c r="B14" s="44" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="8">
@@ -1498,7 +1509,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1511,39 +1522,39 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="22" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
+    </row>
+    <row r="17" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19">
+        <v>45797</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-    </row>
-    <row r="17" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="45">
-        <v>45797</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="7">
         <v>2.5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="21"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="24"/>
       <c r="D18" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="8">
@@ -1551,27 +1562,27 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="21"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="24"/>
       <c r="D20" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="21"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="24"/>
       <c r="D21" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
@@ -1584,39 +1595,39 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
     </row>
     <row r="24" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="31">
+      <c r="A24" s="30">
         <v>45798</v>
       </c>
-      <c r="B24" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="34"/>
+      <c r="B24" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="22"/>
       <c r="D24" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="21"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="24"/>
       <c r="D25" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="19"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="8">
@@ -1624,37 +1635,37 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="19"/>
-      <c r="B27" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="21"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="24"/>
       <c r="D27" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="21"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="24"/>
       <c r="D28" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="21"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="24"/>
       <c r="D29" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="19"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
@@ -1666,391 +1677,487 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="19"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="24"/>
-    </row>
-    <row r="32" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="31">
+    <row r="31" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="20"/>
+      <c r="B31" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="30">
         <v>45799</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="8"/>
+      <c r="B32" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="20"/>
+      <c r="B33" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="19"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="19"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="8"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="20"/>
+      <c r="B35" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="47"/>
+      <c r="D35" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="20"/>
+      <c r="B36" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="47"/>
+      <c r="D36" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="19"/>
-      <c r="B37" s="2" t="s">
+      <c r="A37" s="20"/>
+      <c r="B37" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="24"/>
+      <c r="D37" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="20"/>
+      <c r="B38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="9">
-        <f>SUM(D32:D36)</f>
+      <c r="D38" s="9">
+        <f>SUM(D32:D37)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="34"/>
+    </row>
+    <row r="40" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="30">
+        <v>45800</v>
+      </c>
+      <c r="B40" s="21"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="20"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="20"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="20"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="20"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="20"/>
+      <c r="B45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="9">
+        <f>SUM(D40:D44)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="32"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="30"/>
-    </row>
-    <row r="39" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="31">
-        <v>45800</v>
-      </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="8"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="19"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="8"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="19"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="19"/>
-      <c r="B44" s="2" t="s">
+    <row r="46" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="31"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="34"/>
+    </row>
+    <row r="47" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="30">
+        <v>45803</v>
+      </c>
+      <c r="B47" s="21"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="20"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="20"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="20"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="20"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="20"/>
+      <c r="B52" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="9">
-        <f>SUM(D39:D43)</f>
+      <c r="D52" s="9">
+        <f>SUM(D47:D51)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="32"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="30"/>
-    </row>
-    <row r="46" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="31">
-        <v>45803</v>
-      </c>
-      <c r="B46" s="33"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="19"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="8"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="19"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="19"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="8"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="19"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="19"/>
-      <c r="B51" s="2" t="s">
+    <row r="53" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="31"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="34"/>
+    </row>
+    <row r="54" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="30">
+        <v>45804</v>
+      </c>
+      <c r="B54" s="21"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="20"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="20"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="20"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="20"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="20"/>
+      <c r="B59" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="9">
-        <f>SUM(D46:D50)</f>
+      <c r="D59" s="9">
+        <f>SUM(D54:D58)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="32"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="30"/>
-    </row>
-    <row r="53" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="31">
-        <v>45804</v>
-      </c>
-      <c r="B53" s="33"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="19"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="8"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="19"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="8"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="19"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="8"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="19"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="8"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="19"/>
-      <c r="B58" s="2" t="s">
+    <row r="60" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="31"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="34"/>
+    </row>
+    <row r="61" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="30">
+        <v>45805</v>
+      </c>
+      <c r="B61" s="21"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="7"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="20"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="8"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="20"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="20"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="20"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="8"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="20"/>
+      <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="9">
-        <f>SUM(D53:D57)</f>
+      <c r="D66" s="9">
+        <f>SUM(D61:D65)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="32"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="30"/>
-    </row>
-    <row r="60" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="31">
-        <v>45805</v>
-      </c>
-      <c r="B60" s="33"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="7"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="19"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="8"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="19"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="8"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="19"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="8"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="19"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="8"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="19"/>
-      <c r="B65" s="2" t="s">
+    <row r="67" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="31"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="34"/>
+    </row>
+    <row r="68" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="30">
+        <v>45807</v>
+      </c>
+      <c r="B68" s="21"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="20"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="20"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="8"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="20"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="8"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="20"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="8"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="20"/>
+      <c r="B73" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="9">
-        <f>SUM(D60:D64)</f>
+      <c r="D73" s="9">
+        <f>SUM(D68:D72)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="32"/>
-      <c r="B66" s="28"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="30"/>
-    </row>
-    <row r="67" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="31">
-        <v>45807</v>
-      </c>
-      <c r="B67" s="33"/>
-      <c r="C67" s="34"/>
-      <c r="D67" s="7"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="19"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="8"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="19"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="8"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="19"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="8"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="19"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="8"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="19"/>
-      <c r="B72" s="2" t="s">
+    <row r="74" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="20"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="29"/>
+    </row>
+    <row r="75" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="30">
+        <v>45810</v>
+      </c>
+      <c r="B75" s="21"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="20"/>
+      <c r="B76" s="23"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="8"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="20"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="20"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="8"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="20"/>
+      <c r="B79" s="23"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="8"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="20"/>
+      <c r="B80" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C80" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D72" s="9">
-        <f>SUM(D67:D71)</f>
+      <c r="D80" s="9">
+        <f>SUM(D75:D79)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="19"/>
-      <c r="B73" s="22"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="24"/>
-    </row>
-    <row r="74" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="31">
-        <v>45810</v>
-      </c>
-      <c r="B74" s="33"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="7"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="19"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="8"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="19"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="21"/>
-      <c r="D76" s="8"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="19"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="8"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="19"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="8"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="19"/>
-      <c r="B79" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D79" s="9">
-        <f>SUM(D74:D78)</f>
+    <row r="81" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="31"/>
+      <c r="B81" s="32"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="34"/>
+    </row>
+    <row r="82" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="11"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="12">
+        <f>D15+D22+D30+D38+D45+D52+D59+D66+D73+D80</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="32"/>
-      <c r="B80" s="28"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="30"/>
-    </row>
-    <row r="81" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="11"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D81" s="12">
-        <f>D15+D22+D30+D37+D44+D51+D58+D65+D72+D79</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B82" s="44"/>
-      <c r="C82" s="44"/>
-      <c r="D82" s="44"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="79">
-    <mergeCell ref="A82:D82"/>
+  <mergeCells count="80">
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A7:A16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A75:A81"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="A61:A67"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="A47:A53"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="A40:A46"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A83:D83"/>
     <mergeCell ref="A17:A23"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
@@ -2058,156 +2165,85 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="A32:A38"/>
+    <mergeCell ref="A32:A39"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="A39:A45"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B5:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="A67:A73"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A74:A80"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A7:A16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D15 D24:D30">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Terminé">
+  <conditionalFormatting sqref="D7:D15 D24:D30 D32:D38">
+    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="24" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="16" priority="24" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:D22">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32:D37">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D32)))</formula>
+  <conditionalFormatting sqref="D40:D45">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D32)))</formula>
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D40)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D44">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D39)))</formula>
+  <conditionalFormatting sqref="D47:D52">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D39)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D46:D51">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D46)))</formula>
+  <conditionalFormatting sqref="D54:D59">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D46)))</formula>
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53:D58">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D53)))</formula>
+  <conditionalFormatting sqref="D61:D66">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D61)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D53)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D61)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D65">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D60)))</formula>
+  <conditionalFormatting sqref="D68:D73">
+    <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D60)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="16" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D68)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D67:D72">
-    <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D67)))</formula>
+  <conditionalFormatting sqref="D75:D80">
+    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D75)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="16" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D67)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D75)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D74:D79">
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D74)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D74)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D81">
+  <conditionalFormatting sqref="D82">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D81)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Terminé",D82)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D81)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -2219,8 +2255,8 @@
     <oddFooter>&amp;L&amp;8&amp;F&amp;R&amp;8Page &amp;P/&amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="52" max="16383" man="1"/>
-    <brk id="81" max="3" man="1"/>
+    <brk id="53" max="16383" man="1"/>
+    <brk id="82" max="3" man="1"/>
   </rowBreaks>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>

</xml_diff>